<commit_message>
update api upload, download file
</commit_message>
<xml_diff>
--- a/file-stores/public/products/thanh-toan-hoa-don.xlsx
+++ b/file-stores/public/products/thanh-toan-hoa-don.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\my-project\uaa\file-stores\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\my-project\uaa\file-stores\public\products\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FF3BB2B-63A7-4522-BCBB-BE9E521C512E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B2B42D-39A4-4F7B-AAC2-C9AE8D1B3C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{4443FDD8-481B-4621-9C21-39429EADFA8D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4443FDD8-481B-4621-9C21-39429EADFA8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,16 +25,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>THANH TOÁN HÓA ĐƠN</t>
+  </si>
+  <si>
+    <t>Đơn giá</t>
+  </si>
+  <si>
+    <t>Mã giao dịch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -51,12 +57,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="48"/>
+      <sz val="24"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF0070C0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -85,12 +96,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -407,334 +421,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4AC1493-4C78-4D99-B6E0-C9E3D3B6CF76}">
-  <dimension ref="A1:S15"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:S15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="45.5546875" customWidth="1"/>
+    <col min="2" max="2" width="38.77734375" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
+      <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
+    <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:S15"/>
+    <mergeCell ref="A1:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>